<commit_message>
chore: sample csv change
</commit_message>
<xml_diff>
--- a/client/public/samplecsv.xlsx
+++ b/client/public/samplecsv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maity\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D31C6A9-1017-48BF-AB99-EFB77B86D7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737FE497-AFDC-437B-8A81-0B9032EDB424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="107">
   <si>
     <t>Hotel Name</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Booking Status</t>
-  </si>
-  <si>
-    <t>Modified Date</t>
   </si>
   <si>
     <t>Plan</t>
@@ -379,8 +376,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,21 +718,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9" customWidth="1"/>
+    <col min="1" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="8" width="9" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="11" max="11" width="16.125" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="17" max="17" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,37 +790,34 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1">
+        <v>45385</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
       </c>
       <c r="J2">
         <v>5000</v>
@@ -828,57 +826,54 @@
         <v>1500</v>
       </c>
       <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
       </c>
       <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" t="s">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>37</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
       </c>
       <c r="J3">
         <v>4032</v>
@@ -887,57 +882,54 @@
         <v>1200</v>
       </c>
       <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
       <c r="N3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" t="s">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" t="s">
-        <v>43</v>
       </c>
       <c r="J4">
         <v>3024</v>
@@ -946,57 +938,54 @@
         <v>1000</v>
       </c>
       <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
         <v>28</v>
       </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
       <c r="N4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="s">
         <v>39</v>
       </c>
-      <c r="O4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
-      </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>4032</v>
@@ -1005,57 +994,54 @@
         <v>1200</v>
       </c>
       <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" t="s">
-        <v>29</v>
-      </c>
       <c r="N5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
         <v>39</v>
       </c>
-      <c r="O5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6">
         <v>5000</v>
@@ -1064,57 +1050,54 @@
         <v>1500</v>
       </c>
       <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
         <v>28</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>29</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>30</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>31</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>32</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>28</v>
       </c>
       <c r="R6" t="s">
         <v>33</v>
       </c>
-      <c r="S6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
         <v>58</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
         <v>60</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" t="s">
-        <v>61</v>
       </c>
       <c r="J7">
         <v>12880</v>
@@ -1123,57 +1106,54 @@
         <v>4000</v>
       </c>
       <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
         <v>28</v>
       </c>
-      <c r="M7" t="s">
-        <v>29</v>
-      </c>
       <c r="N7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
         <v>31</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>32</v>
       </c>
-      <c r="Q7" t="s">
-        <v>28</v>
-      </c>
       <c r="R7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
         <v>63</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8">
         <v>5796</v>
@@ -1182,57 +1162,54 @@
         <v>1500</v>
       </c>
       <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" t="s">
         <v>28</v>
       </c>
-      <c r="M8" t="s">
-        <v>29</v>
-      </c>
       <c r="N8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" t="s">
         <v>39</v>
       </c>
-      <c r="O8" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" t="s">
-        <v>33</v>
-      </c>
-      <c r="S8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
       <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
+      <c r="F9" s="1">
+        <v>45629</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9">
         <v>5039</v>
@@ -1241,57 +1218,54 @@
         <v>1500</v>
       </c>
       <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
         <v>28</v>
       </c>
-      <c r="M9" t="s">
-        <v>29</v>
-      </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
         <v>31</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" t="s">
-        <v>28</v>
-      </c>
       <c r="R9" t="s">
-        <v>33</v>
-      </c>
-      <c r="S9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J10">
         <v>2800</v>
@@ -1300,57 +1274,54 @@
         <v>1500</v>
       </c>
       <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
         <v>28</v>
       </c>
-      <c r="M10" t="s">
-        <v>29</v>
-      </c>
       <c r="N10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" t="s">
         <v>39</v>
       </c>
-      <c r="O10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P10" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
         <v>70</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>71</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" t="s">
         <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" t="s">
-        <v>73</v>
       </c>
       <c r="J11">
         <v>12000</v>
@@ -1359,57 +1330,54 @@
         <v>3500</v>
       </c>
       <c r="L11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
         <v>29</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>30</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>31</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>32</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>28</v>
       </c>
       <c r="R11" t="s">
         <v>33</v>
       </c>
-      <c r="S11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
         <v>74</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
         <v>75</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" t="s">
-        <v>77</v>
-      </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" t="s">
         <v>46</v>
-      </c>
-      <c r="I12" t="s">
-        <v>47</v>
       </c>
       <c r="J12">
         <v>8624</v>
@@ -1418,57 +1386,54 @@
         <v>2310</v>
       </c>
       <c r="L12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" t="s">
         <v>39</v>
       </c>
-      <c r="O12" t="s">
-        <v>31</v>
-      </c>
-      <c r="P12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" t="s">
-        <v>33</v>
-      </c>
-      <c r="S12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
       <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>23</v>
       </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J13">
         <v>7000</v>
@@ -1477,57 +1442,54 @@
         <v>2000</v>
       </c>
       <c r="L13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" t="s">
         <v>29</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>30</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>31</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>32</v>
       </c>
-      <c r="Q13" t="s">
-        <v>28</v>
-      </c>
       <c r="R13" t="s">
-        <v>33</v>
-      </c>
-      <c r="S13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>81</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" t="s">
         <v>82</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" t="s">
-        <v>83</v>
       </c>
       <c r="J14">
         <v>12550</v>
@@ -1536,57 +1498,54 @@
         <v>4000</v>
       </c>
       <c r="L14" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
         <v>84</v>
       </c>
-      <c r="M14" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" t="s">
-        <v>31</v>
-      </c>
-      <c r="P14" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" t="s">
-        <v>33</v>
-      </c>
-      <c r="S14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>85</v>
       </c>
-      <c r="C15" t="s">
-        <v>86</v>
-      </c>
       <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" t="s">
         <v>46</v>
-      </c>
-      <c r="I15" t="s">
-        <v>47</v>
       </c>
       <c r="J15">
         <v>6400</v>
@@ -1595,57 +1554,54 @@
         <v>2000</v>
       </c>
       <c r="L15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
         <v>29</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>30</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>31</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>32</v>
       </c>
-      <c r="Q15" t="s">
-        <v>28</v>
-      </c>
       <c r="R15" t="s">
-        <v>33</v>
-      </c>
-      <c r="S15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
         <v>87</v>
       </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16">
         <v>7000</v>
@@ -1654,57 +1610,54 @@
         <v>3500</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" t="s">
         <v>29</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>30</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>31</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>32</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>28</v>
       </c>
       <c r="R16" t="s">
         <v>33</v>
       </c>
-      <c r="S16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
         <v>89</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17" t="s">
         <v>91</v>
-      </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" t="s">
-        <v>92</v>
       </c>
       <c r="J17">
         <v>10800</v>
@@ -1713,57 +1666,54 @@
         <v>3000</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
         <v>29</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>30</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>31</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>32</v>
       </c>
-      <c r="Q17" t="s">
-        <v>28</v>
-      </c>
       <c r="R17" t="s">
-        <v>33</v>
-      </c>
-      <c r="S17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>94</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
         <v>95</v>
       </c>
-      <c r="D18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" t="s">
-        <v>96</v>
-      </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18">
         <v>5000</v>
@@ -1772,57 +1722,54 @@
         <v>1500</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M18" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" t="s">
         <v>29</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>30</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>31</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>32</v>
       </c>
-      <c r="Q18" t="s">
-        <v>28</v>
-      </c>
       <c r="R18" t="s">
-        <v>33</v>
-      </c>
-      <c r="S18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>98</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" t="s">
         <v>99</v>
       </c>
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>100</v>
-      </c>
-      <c r="I19" t="s">
-        <v>101</v>
       </c>
       <c r="J19">
         <v>14000</v>
@@ -1831,57 +1778,54 @@
         <v>4200</v>
       </c>
       <c r="L19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" t="s">
         <v>29</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>30</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>31</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>32</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>28</v>
       </c>
       <c r="R19" t="s">
         <v>33</v>
       </c>
-      <c r="S19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
         <v>102</v>
       </c>
-      <c r="C20" t="s">
-        <v>103</v>
-      </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J20">
         <v>16500</v>
@@ -1890,57 +1834,54 @@
         <v>11247</v>
       </c>
       <c r="L20" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>32</v>
+      </c>
+      <c r="R20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
         <v>104</v>
       </c>
-      <c r="M20" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" t="s">
-        <v>30</v>
-      </c>
-      <c r="O20" t="s">
-        <v>31</v>
-      </c>
-      <c r="P20" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>28</v>
-      </c>
-      <c r="R20" t="s">
-        <v>33</v>
-      </c>
-      <c r="S20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>105</v>
       </c>
-      <c r="C21" t="s">
-        <v>106</v>
-      </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
         <v>59</v>
       </c>
-      <c r="F21" t="s">
-        <v>60</v>
-      </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J21">
         <v>5318</v>
@@ -1949,34 +1890,31 @@
         <v>1595</v>
       </c>
       <c r="L21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N21" t="s">
+        <v>38</v>
+      </c>
+      <c r="O21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>32</v>
+      </c>
+      <c r="R21" t="s">
         <v>39</v>
-      </c>
-      <c r="O21" t="s">
-        <v>31</v>
-      </c>
-      <c r="P21" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>28</v>
-      </c>
-      <c r="R21" t="s">
-        <v>33</v>
-      </c>
-      <c r="S21" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K6 L1:S6 A7:K21 L7:S21" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:K1 L1:P6 A7:K8 L7:P21 Q1:R6 Q7:R21 A3:K6 A2:E2 G2:K2 A10:K21 A9:E9 G9:K9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>